<commit_message>
Updates for having reference programs fixed
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Tanzania/2018Jan/InputForCode_Tanzania.xlsx
+++ b/input_spreadsheets/Tanzania/2018Jan/InputForCode_Tanzania.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-36100" yWindow="-19860" windowWidth="34820" windowHeight="21140" tabRatio="888" firstSheet="17" activeTab="21"/>
+    <workbookView xWindow="-36600" yWindow="-21140" windowWidth="34820" windowHeight="21140" tabRatio="888" firstSheet="19" activeTab="26"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,8 @@
     <sheet name="Program risk areas" sheetId="36" r:id="rId25"/>
     <sheet name="Population risk areas" sheetId="43" r:id="rId26"/>
     <sheet name="Programs cost and coverage" sheetId="20" r:id="rId27"/>
-    <sheet name="Programs to include" sheetId="44" r:id="rId28"/>
+    <sheet name="Reference programs" sheetId="49" r:id="rId28"/>
+    <sheet name="Programs to include" sheetId="44" r:id="rId29"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -2632,6 +2633,40 @@
 </comments>
 </file>
 
+<file path=xl/comments21.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Sam</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Programs whose coverage cannot fall below baseline %</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
@@ -3355,7 +3390,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1293" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1302" uniqueCount="271">
   <si>
     <t>year</t>
   </si>
@@ -4537,7 +4572,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="675">
+  <cellStyleXfs count="689">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4549,6 +4584,20 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5449,7 +5498,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="675">
+  <cellStyles count="689">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -5787,6 +5836,13 @@
     <cellStyle name="Followed Hyperlink" xfId="670" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="672" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="674" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="676" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="678" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="680" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="682" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="684" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="686" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="688" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6123,6 +6179,13 @@
     <cellStyle name="Hyperlink" xfId="669" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="671" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="673" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="675" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="677" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="679" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="681" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="683" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="685" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="687" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
@@ -14087,8 +14150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="135" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView zoomScale="135" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -16205,7 +16268,8 @@
         <v>78</v>
       </c>
       <c r="C49" s="31">
-        <v>0.1</v>
+        <f>'Baseline year demographics'!$C9</f>
+        <v>1</v>
       </c>
       <c r="D49" s="31">
         <f>'Baseline year demographics'!$C9</f>
@@ -18898,8 +18962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -19204,8 +19268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -20048,8 +20112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -20852,11 +20916,77 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P43" sqref="P43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="53" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="B1" s="10"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>258</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Objective & budget update for optimisation
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Tanzania/2018Jan/InputForCode_Tanzania.xlsx
+++ b/input_spreadsheets/Tanzania/2018Jan/InputForCode_Tanzania.xlsx
@@ -7490,7 +7490,7 @@
   <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -14151,7 +14151,7 @@
   <dimension ref="A1:O53"/>
   <sheetViews>
     <sheetView zoomScale="135" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -20113,7 +20113,7 @@
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Changed to run for all programs
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Tanzania/2018Jan/InputForCode_Tanzania.xlsx
+++ b/input_spreadsheets/Tanzania/2018Jan/InputForCode_Tanzania.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/input_spreadsheets/Tanzania/2018Jan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0840120B-D4A2-DE48-997B-BC3CA80CD04F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B19FA1C-E330-B740-BBF9-84D981B87C98}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6180" yWindow="-21140" windowWidth="19200" windowHeight="21140" tabRatio="888" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6180" yWindow="-21140" windowWidth="19200" windowHeight="21140" tabRatio="888" firstSheet="10" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -3461,7 +3461,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1483" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1514" uniqueCount="290">
   <si>
     <t>year</t>
   </si>
@@ -7764,7 +7764,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -12832,8 +12832,8 @@
   </sheetPr>
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -13044,10 +13044,10 @@
         <v>1</v>
       </c>
       <c r="F12" s="4">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="G12" s="4">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
@@ -14365,6 +14365,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B33"/>
@@ -14375,11 +14380,6 @@
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B22:B24"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -27466,7 +27466,7 @@
   <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -27495,21 +27495,33 @@
       <c r="A3" s="120" t="s">
         <v>268</v>
       </c>
+      <c r="B3" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
         <v>264</v>
       </c>
+      <c r="B4" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
         <v>143</v>
       </c>
+      <c r="B5" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>185</v>
       </c>
+      <c r="B6" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" s="12" t="s">
@@ -27523,81 +27535,129 @@
       <c r="A8" s="12" t="s">
         <v>146</v>
       </c>
+      <c r="B8" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" s="12" t="s">
         <v>144</v>
       </c>
+      <c r="B9" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>124</v>
       </c>
+      <c r="B10" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>132</v>
       </c>
+      <c r="B11" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>125</v>
       </c>
+      <c r="B12" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>133</v>
       </c>
+      <c r="B13" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>126</v>
       </c>
+      <c r="B14" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>134</v>
       </c>
+      <c r="B15" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>123</v>
       </c>
+      <c r="B16" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>131</v>
       </c>
+      <c r="B17" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>121</v>
       </c>
+      <c r="B18" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>129</v>
       </c>
+      <c r="B19" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>122</v>
       </c>
+      <c r="B20" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>130</v>
       </c>
+      <c r="B21" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>120</v>
       </c>
+      <c r="B22" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>128</v>
       </c>
+      <c r="B23" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
@@ -27611,11 +27671,17 @@
       <c r="A25" s="4" t="s">
         <v>77</v>
       </c>
+      <c r="B25" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
         <v>139</v>
       </c>
+      <c r="B26" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
@@ -27652,26 +27718,41 @@
       <c r="A32" s="4" t="s">
         <v>266</v>
       </c>
+      <c r="B32" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A33" s="4" t="s">
         <v>265</v>
       </c>
+      <c r="B33" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>135</v>
       </c>
+      <c r="B34" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>138</v>
       </c>
+      <c r="B35" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>262</v>
       </c>
+      <c r="B36" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A37" s="4" t="s">
@@ -27685,16 +27766,25 @@
       <c r="A38" s="4" t="s">
         <v>75</v>
       </c>
+      <c r="B38" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A39" s="4" t="s">
         <v>136</v>
       </c>
+      <c r="B39" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="s">
         <v>74</v>
       </c>
+      <c r="B40" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A41" s="29" t="s">
@@ -27732,7 +27822,7 @@
       <c r="A45" t="s">
         <v>261</v>
       </c>
-      <c r="B45" s="133" t="s">
+      <c r="B45" t="s">
         <v>165</v>
       </c>
     </row>
@@ -27740,7 +27830,7 @@
       <c r="A46" t="s">
         <v>260</v>
       </c>
-      <c r="B46" s="133" t="s">
+      <c r="B46" t="s">
         <v>165</v>
       </c>
     </row>
@@ -27748,7 +27838,7 @@
       <c r="A47" t="s">
         <v>259</v>
       </c>
-      <c r="B47" s="133" t="s">
+      <c r="B47" t="s">
         <v>165</v>
       </c>
     </row>
@@ -27756,7 +27846,7 @@
       <c r="A48" t="s">
         <v>257</v>
       </c>
-      <c r="B48" s="133" t="s">
+      <c r="B48" t="s">
         <v>165</v>
       </c>
     </row>
@@ -27764,7 +27854,7 @@
       <c r="A49" t="s">
         <v>258</v>
       </c>
-      <c r="B49" s="133" t="s">
+      <c r="B49" t="s">
         <v>165</v>
       </c>
     </row>
@@ -27779,6 +27869,9 @@
     <row r="51" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A51" s="4" t="s">
         <v>140</v>
+      </c>
+      <c r="B51" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Updated for all progs (not outside malaria area due to area==1)
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Tanzania/2018Jan/InputForCode_Tanzania.xlsx
+++ b/input_spreadsheets/Tanzania/2018Jan/InputForCode_Tanzania.xlsx
@@ -8,10 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/input_spreadsheets/Tanzania/2018Jan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3CEF5C3-7117-1D48-9B6F-37BC7F561BC5}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA07A42-C2C9-A240-9928-FAE9E0FEACAD}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6180" yWindow="-21140" windowWidth="19200" windowHeight="21140" tabRatio="888" firstSheet="27" activeTab="28" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="13020" yWindow="-21140" windowWidth="19200" windowHeight="21140" firstSheet="26" activeTab="31" xr2:uid="{9CA16DF4-3AE6-9240-921D-580CF0357D1B}"/>
+    <workbookView xWindow="1740" yWindow="-21140" windowWidth="30480" windowHeight="21140" firstSheet="25" activeTab="31" xr2:uid="{9CA16DF4-3AE6-9240-921D-580CF0357D1B}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -3462,7 +3461,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1484" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1500" uniqueCount="290">
   <si>
     <t>year</t>
   </si>
@@ -7766,9 +7765,8 @@
   <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -8206,10 +8204,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -8778,10 +8773,7 @@
   </sheetPr>
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D96" sqref="D96"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -12836,10 +12828,7 @@
   </sheetPr>
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -13268,10 +13257,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -14371,6 +14357,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B33"/>
@@ -14381,11 +14372,6 @@
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B22:B24"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -14396,10 +14382,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView zoomScale="133" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -14612,10 +14595,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:D12"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -14808,10 +14788,7 @@
   </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -14886,10 +14863,7 @@
   </sheetPr>
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -15195,10 +15169,7 @@
   </sheetPr>
   <dimension ref="A1:O43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -16655,10 +16626,7 @@
   </sheetPr>
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -16744,10 +16712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -17397,10 +17362,7 @@
   </sheetPr>
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -18605,10 +18567,7 @@
   </sheetPr>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -18813,10 +18772,7 @@
   </sheetPr>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -18990,10 +18946,7 @@
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -19068,10 +19021,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" zoomScale="135" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -21459,10 +21411,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:O56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -23882,10 +23831,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -24189,10 +24135,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -24746,10 +24689,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -25035,10 +24975,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView topLeftCell="A2" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -25823,10 +25760,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{732C9C65-1200-044E-9799-D4D48ED0657E}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -26283,10 +26217,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60F5240D-F5E2-7843-8F74-E64484849FE7}">
   <dimension ref="A1:P107"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
@@ -27424,10 +27355,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P43" sqref="P43"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -27491,11 +27419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
-    </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -27516,7 +27441,7 @@
       <c r="A2" t="s">
         <v>55</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="133" t="s">
         <v>165</v>
       </c>
     </row>
@@ -27524,21 +27449,31 @@
       <c r="A3" s="120" t="s">
         <v>268</v>
       </c>
+      <c r="B3" s="133"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
         <v>264</v>
       </c>
+      <c r="B4" s="133" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
         <v>143</v>
       </c>
+      <c r="B5" s="133" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>185</v>
       </c>
+      <c r="B6" s="133" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" s="12" t="s">
@@ -27552,81 +27487,111 @@
       <c r="A8" s="12" t="s">
         <v>146</v>
       </c>
+      <c r="B8" s="133"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" s="12" t="s">
         <v>144</v>
       </c>
+      <c r="B9" s="133"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>124</v>
       </c>
+      <c r="B10" s="133"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>132</v>
       </c>
+      <c r="B11" s="133" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>125</v>
       </c>
+      <c r="B12" s="133"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>133</v>
       </c>
+      <c r="B13" s="133" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>126</v>
       </c>
+      <c r="B14" s="133"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>134</v>
       </c>
+      <c r="B15" s="133" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>123</v>
       </c>
+      <c r="B16" s="133"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>131</v>
       </c>
+      <c r="B17" s="133" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>121</v>
       </c>
+      <c r="B18" s="133"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>129</v>
       </c>
+      <c r="B19" s="133" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>122</v>
       </c>
+      <c r="B20" s="133"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>130</v>
       </c>
+      <c r="B21" s="133" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>120</v>
       </c>
+      <c r="B22" s="133"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>128</v>
       </c>
+      <c r="B23" s="133" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
@@ -27640,11 +27605,15 @@
       <c r="A25" s="4" t="s">
         <v>77</v>
       </c>
+      <c r="B25" s="133"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
         <v>139</v>
       </c>
+      <c r="B26" s="133" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
@@ -27681,11 +27650,17 @@
       <c r="A32" s="4" t="s">
         <v>266</v>
       </c>
+      <c r="B32" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A33" s="4" t="s">
         <v>265</v>
       </c>
+      <c r="B33" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
@@ -27704,6 +27679,9 @@
       <c r="A36" t="s">
         <v>262</v>
       </c>
+      <c r="B36" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A37" s="4" t="s">
@@ -27722,6 +27700,9 @@
       <c r="A39" s="4" t="s">
         <v>136</v>
       </c>
+      <c r="B39" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="s">
@@ -27811,6 +27792,9 @@
     <row r="51" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A51" s="4" t="s">
         <v>140</v>
+      </c>
+      <c r="B51" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.15">
@@ -27840,10 +27824,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -28761,10 +28742,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
@@ -28909,10 +28887,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -29275,10 +29250,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -29663,10 +29635,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDDF9271-A6AF-7E41-A1A9-AAF3090BE398}">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
@@ -30083,10 +30052,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C15"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>

</xml_diff>

<commit_message>
New objectives for subset case
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Tanzania/2018Jan/InputForCode_Tanzania.xlsx
+++ b/input_spreadsheets/Tanzania/2018Jan/InputForCode_Tanzania.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/input_spreadsheets/Tanzania/2018Jan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA07A42-C2C9-A240-9928-FAE9E0FEACAD}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC034B1-3289-A246-88CF-C401AA3E6B9E}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="-21140" windowWidth="30480" windowHeight="21140" firstSheet="25" activeTab="31" xr2:uid="{9CA16DF4-3AE6-9240-921D-580CF0357D1B}"/>
+    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="19200" windowHeight="21140" firstSheet="22" activeTab="31" xr2:uid="{9CA16DF4-3AE6-9240-921D-580CF0357D1B}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -3461,7 +3461,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1500" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1483" uniqueCount="290">
   <si>
     <t>year</t>
   </si>
@@ -14357,11 +14357,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B33"/>
@@ -14372,6 +14367,11 @@
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -14863,7 +14863,9 @@
   </sheetPr>
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -15169,7 +15171,9 @@
   </sheetPr>
   <dimension ref="A1:O43"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -19022,7 +19026,7 @@
   <dimension ref="A1:O53"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -21411,7 +21415,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:O56"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -23831,7 +23837,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:XFD31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -23964,7 +23972,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>128</v>
       </c>
@@ -24135,7 +24143,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -27420,7 +27430,7 @@
   <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -27455,25 +27465,19 @@
       <c r="A4" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="B4" s="133" t="s">
-        <v>165</v>
-      </c>
+      <c r="B4" s="133"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B5" s="133" t="s">
-        <v>165</v>
-      </c>
+      <c r="B5" s="133"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>185</v>
       </c>
-      <c r="B6" s="133" t="s">
-        <v>165</v>
-      </c>
+      <c r="B6" s="133"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" s="12" t="s">
@@ -27505,9 +27509,7 @@
       <c r="A11" t="s">
         <v>132</v>
       </c>
-      <c r="B11" s="133" t="s">
-        <v>165</v>
-      </c>
+      <c r="B11" s="133"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
@@ -27519,9 +27521,7 @@
       <c r="A13" t="s">
         <v>133</v>
       </c>
-      <c r="B13" s="133" t="s">
-        <v>165</v>
-      </c>
+      <c r="B13" s="133"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
@@ -27533,9 +27533,7 @@
       <c r="A15" t="s">
         <v>134</v>
       </c>
-      <c r="B15" s="133" t="s">
-        <v>165</v>
-      </c>
+      <c r="B15" s="133"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
@@ -27547,9 +27545,7 @@
       <c r="A17" t="s">
         <v>131</v>
       </c>
-      <c r="B17" s="133" t="s">
-        <v>165</v>
-      </c>
+      <c r="B17" s="133"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
@@ -27561,9 +27557,7 @@
       <c r="A19" t="s">
         <v>129</v>
       </c>
-      <c r="B19" s="133" t="s">
-        <v>165</v>
-      </c>
+      <c r="B19" s="133"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
@@ -27575,9 +27569,7 @@
       <c r="A21" t="s">
         <v>130</v>
       </c>
-      <c r="B21" s="133" t="s">
-        <v>165</v>
-      </c>
+      <c r="B21" s="133"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
@@ -27589,9 +27581,7 @@
       <c r="A23" t="s">
         <v>128</v>
       </c>
-      <c r="B23" s="133" t="s">
-        <v>165</v>
-      </c>
+      <c r="B23" s="133"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
@@ -27611,9 +27601,7 @@
       <c r="A26" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B26" s="133" t="s">
-        <v>165</v>
-      </c>
+      <c r="B26" s="133"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
@@ -27650,17 +27638,11 @@
       <c r="A32" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="B32" t="s">
-        <v>165</v>
-      </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A33" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="B33" t="s">
-        <v>165</v>
-      </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
@@ -27671,17 +27653,11 @@
       <c r="A35" t="s">
         <v>138</v>
       </c>
-      <c r="B35" t="s">
-        <v>165</v>
-      </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>262</v>
       </c>
-      <c r="B36" t="s">
-        <v>165</v>
-      </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A37" s="4" t="s">
@@ -27700,9 +27676,6 @@
       <c r="A39" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="B39" t="s">
-        <v>165</v>
-      </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="s">
@@ -27792,9 +27765,6 @@
     <row r="51" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A51" s="4" t="s">
         <v>140</v>
-      </c>
-      <c r="B51" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Updated family planning target pop
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Tanzania/2018Jan/InputForCode_Tanzania.xlsx
+++ b/input_spreadsheets/Tanzania/2018Jan/InputForCode_Tanzania.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/input_spreadsheets/Tanzania/2018Jan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B5DBB90-02AF-BC4B-9A92-7FFCDAEA0975}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B76FECA5-E8FB-834C-8353-98652BDFCF68}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="19200" windowHeight="21140" firstSheet="28" activeTab="31" xr2:uid="{9CA16DF4-3AE6-9240-921D-580CF0357D1B}"/>
+    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="31540" windowHeight="21140" firstSheet="16" activeTab="23" xr2:uid="{9CA16DF4-3AE6-9240-921D-580CF0357D1B}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -7765,7 +7765,7 @@
   <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -19025,8 +19025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="O36" sqref="O36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -20624,16 +20624,20 @@
         <v>0</v>
       </c>
       <c r="L36" s="109">
-        <v>1</v>
+        <f>'Programs cost and coverage'!$B6+'Baseline year demographics'!$C12</f>
+        <v>0.221</v>
       </c>
       <c r="M36" s="109">
-        <v>1</v>
+        <f>'Programs cost and coverage'!$B6+'Baseline year demographics'!$C12</f>
+        <v>0.221</v>
       </c>
       <c r="N36" s="109">
-        <v>1</v>
+        <f>'Programs cost and coverage'!$B6+'Baseline year demographics'!$C12</f>
+        <v>0.221</v>
       </c>
       <c r="O36" s="109">
-        <v>1</v>
+        <f>'Programs cost and coverage'!$B6+'Baseline year demographics'!$C12</f>
+        <v>0.221</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -23837,8 +23841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:XFD31"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -24985,7 +24989,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -26227,7 +26233,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60F5240D-F5E2-7843-8F74-E64484849FE7}">
   <dimension ref="A1:P107"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
@@ -27365,7 +27373,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -27429,8 +27439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Removed IPTp and bender dependencies
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Tanzania/2018Jan/InputForCode_Tanzania.xlsx
+++ b/input_spreadsheets/Tanzania/2018Jan/InputForCode_Tanzania.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/input_spreadsheets/Tanzania/2018Jan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B76FECA5-E8FB-834C-8353-98652BDFCF68}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F43959B-FFF7-D241-938D-B6F205CDD051}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="31540" windowHeight="21140" firstSheet="16" activeTab="23" xr2:uid="{9CA16DF4-3AE6-9240-921D-580CF0357D1B}"/>
+    <workbookView xWindow="0" yWindow="-21140" windowWidth="38400" windowHeight="21140" firstSheet="16" activeTab="25" xr2:uid="{9CA16DF4-3AE6-9240-921D-580CF0357D1B}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -3461,7 +3461,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1500" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1489" uniqueCount="290">
   <si>
     <t>year</t>
   </si>
@@ -14357,11 +14357,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B33"/>
@@ -14372,6 +14367,11 @@
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -19025,7 +19025,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="O36" sqref="O36"/>
     </sheetView>
   </sheetViews>
@@ -23841,8 +23841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -23902,9 +23902,7 @@
       <c r="A9" t="s">
         <v>132</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>78</v>
-      </c>
+      <c r="C9" s="4"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
@@ -23915,9 +23913,7 @@
       <c r="A11" t="s">
         <v>133</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>78</v>
-      </c>
+      <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
@@ -23928,9 +23924,7 @@
       <c r="A13" t="s">
         <v>134</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>78</v>
-      </c>
+      <c r="C13" s="4"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
@@ -23941,9 +23935,7 @@
       <c r="A15" t="s">
         <v>131</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>78</v>
-      </c>
+      <c r="C15" s="4"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
@@ -23954,9 +23946,7 @@
       <c r="A17" t="s">
         <v>129</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>78</v>
-      </c>
+      <c r="C17" s="4"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
@@ -23967,9 +23957,7 @@
       <c r="A19" t="s">
         <v>130</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>78</v>
-      </c>
+      <c r="C19" s="4"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
@@ -23980,9 +23968,7 @@
       <c r="A21" t="s">
         <v>128</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>78</v>
-      </c>
+      <c r="C21" s="4"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
@@ -24004,9 +23990,6 @@
       <c r="B24" t="s">
         <v>138</v>
       </c>
-      <c r="C24" t="s">
-        <v>119</v>
-      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" s="4" t="s">
@@ -24051,9 +24034,6 @@
       <c r="A31" t="s">
         <v>138</v>
       </c>
-      <c r="C31" t="s">
-        <v>119</v>
-      </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="s">
@@ -24072,9 +24052,7 @@
       <c r="A34" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C34" s="4" t="s">
-        <v>78</v>
-      </c>
+      <c r="C34" s="4"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A35" s="4" t="s">
@@ -24091,9 +24069,7 @@
       <c r="B36" t="s">
         <v>136</v>
       </c>
-      <c r="C36" s="4" t="s">
-        <v>78</v>
-      </c>
+      <c r="C36" s="4"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A37" s="4" t="s">

</xml_diff>

<commit_message>
Updated RR data from LiST
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Tanzania/2018Jan/InputForCode_Tanzania.xlsx
+++ b/input_spreadsheets/Tanzania/2018Jan/InputForCode_Tanzania.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/input_spreadsheets/Tanzania/2018Jan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F43959B-FFF7-D241-938D-B6F205CDD051}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F102327-81CE-D44D-A56C-E112B68B557A}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-21140" windowWidth="38400" windowHeight="21140" firstSheet="16" activeTab="25" xr2:uid="{9CA16DF4-3AE6-9240-921D-580CF0357D1B}"/>
+    <workbookView xWindow="0" yWindow="-21140" windowWidth="38400" windowHeight="21140" firstSheet="7" activeTab="10" xr2:uid="{9CA16DF4-3AE6-9240-921D-580CF0357D1B}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -8773,7 +8773,9 @@
   </sheetPr>
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="J61" sqref="J61"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -11163,16 +11165,16 @@
         <v>1</v>
       </c>
       <c r="I57" s="4">
-        <v>3.51</v>
+        <v>10.675000000000001</v>
       </c>
       <c r="J57" s="4">
-        <v>3.51</v>
+        <v>10.675000000000001</v>
       </c>
       <c r="K57" s="4">
-        <v>3.51</v>
+        <v>10.675000000000001</v>
       </c>
       <c r="L57" s="4">
-        <v>3.51</v>
+        <v>10.675000000000001</v>
       </c>
       <c r="M57">
         <v>1</v>
@@ -11254,16 +11256,16 @@
         <v>1</v>
       </c>
       <c r="I59" s="4">
-        <v>3.51</v>
+        <v>10.675000000000001</v>
       </c>
       <c r="J59" s="4">
-        <v>3.51</v>
+        <v>10.675000000000001</v>
       </c>
       <c r="K59" s="4">
-        <v>3.51</v>
+        <v>10.675000000000001</v>
       </c>
       <c r="L59" s="4">
-        <v>3.51</v>
+        <v>10.675000000000001</v>
       </c>
       <c r="M59">
         <v>1</v>
@@ -11345,16 +11347,16 @@
         <v>1</v>
       </c>
       <c r="I61" s="4">
-        <v>3.51</v>
+        <v>10.675000000000001</v>
       </c>
       <c r="J61" s="4">
-        <v>3.51</v>
+        <v>10.675000000000001</v>
       </c>
       <c r="K61" s="4">
-        <v>3.51</v>
+        <v>10.675000000000001</v>
       </c>
       <c r="L61" s="4">
-        <v>3.51</v>
+        <v>10.675000000000001</v>
       </c>
       <c r="M61">
         <v>1</v>
@@ -11428,7 +11430,7 @@
         <v>38</v>
       </c>
       <c r="D65" s="12">
-        <v>2.2799999999999998</v>
+        <v>1.35</v>
       </c>
       <c r="E65" s="4">
         <v>1</v>
@@ -11472,7 +11474,7 @@
         <v>39</v>
       </c>
       <c r="D66" s="12">
-        <v>4.62</v>
+        <v>1.35</v>
       </c>
       <c r="E66" s="4">
         <v>1</v>
@@ -11516,7 +11518,7 @@
         <v>40</v>
       </c>
       <c r="D67" s="12">
-        <v>10.53</v>
+        <v>5.4</v>
       </c>
       <c r="E67" s="4">
         <v>1</v>
@@ -11606,8 +11608,8 @@
       <c r="C69" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D69" s="4">
-        <v>1.66</v>
+      <c r="D69" s="12">
+        <v>1.35</v>
       </c>
       <c r="E69" s="4">
         <v>1</v>
@@ -11650,8 +11652,8 @@
       <c r="C70" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D70" s="4">
-        <v>2.5</v>
+      <c r="D70" s="12">
+        <v>1.35</v>
       </c>
       <c r="E70" s="4">
         <v>1</v>
@@ -11694,8 +11696,8 @@
       <c r="C71" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D71" s="4">
-        <v>14.97</v>
+      <c r="D71" s="12">
+        <v>5.4</v>
       </c>
       <c r="E71" s="4">
         <v>1</v>
@@ -11785,8 +11787,8 @@
       <c r="C73" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D73" s="4">
-        <v>1.66</v>
+      <c r="D73" s="12">
+        <v>1.35</v>
       </c>
       <c r="E73" s="4">
         <v>1</v>
@@ -11829,8 +11831,8 @@
       <c r="C74" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D74" s="4">
-        <v>2.5</v>
+      <c r="D74" s="12">
+        <v>1.35</v>
       </c>
       <c r="E74" s="4">
         <v>1</v>
@@ -11873,8 +11875,8 @@
       <c r="C75" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D75" s="4">
-        <v>14.97</v>
+      <c r="D75" s="12">
+        <v>5.4</v>
       </c>
       <c r="E75" s="4">
         <v>1</v>
@@ -12235,13 +12237,13 @@
         <v>1</v>
       </c>
       <c r="E83" s="12">
-        <v>10.53</v>
+        <v>10.52</v>
       </c>
       <c r="F83" s="11">
-        <v>2.1</v>
+        <v>1.47</v>
       </c>
       <c r="G83" s="11">
-        <v>2.1</v>
+        <v>2.57</v>
       </c>
       <c r="H83" s="11">
         <v>1</v>
@@ -12505,7 +12507,7 @@
         <v>1</v>
       </c>
       <c r="E89">
-        <v>1</v>
+        <v>1.48</v>
       </c>
       <c r="F89">
         <v>1</v>
@@ -12549,7 +12551,7 @@
         <v>1</v>
       </c>
       <c r="E90">
-        <v>1</v>
+        <v>2.84</v>
       </c>
       <c r="F90">
         <v>1</v>
@@ -12593,13 +12595,13 @@
         <v>1</v>
       </c>
       <c r="E91">
-        <v>1</v>
+        <v>14.4</v>
       </c>
       <c r="F91">
-        <v>1</v>
+        <v>3.69</v>
       </c>
       <c r="G91">
-        <v>1</v>
+        <v>3.69</v>
       </c>
       <c r="H91">
         <v>1</v>
@@ -23841,7 +23843,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated wasting incidence effectiveness
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Tanzania/2018Jan/InputForCode_Tanzania.xlsx
+++ b/input_spreadsheets/Tanzania/2018Jan/InputForCode_Tanzania.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/input_spreadsheets/Tanzania/2018Jan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F102327-81CE-D44D-A56C-E112B68B557A}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0CCF695-47AC-7E43-8715-EB9172F164C2}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-21140" windowWidth="38400" windowHeight="21140" firstSheet="7" activeTab="10" xr2:uid="{9CA16DF4-3AE6-9240-921D-580CF0357D1B}"/>
+    <workbookView xWindow="0" yWindow="-21140" windowWidth="38400" windowHeight="21140" firstSheet="14" activeTab="19" xr2:uid="{9CA16DF4-3AE6-9240-921D-580CF0357D1B}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -486,13 +486,46 @@
         </r>
       </text>
     </comment>
+    <comment ref="E13" authorId="0" shapeId="0" xr:uid="{894C6F33-B8E6-8B45-8B5E-FDFEB9A77B85}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nick had these in the params documentation</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0900-000004000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
@@ -501,12 +534,21 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-This assumes we deliver PPCF with education to the poor</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>This assumes we deliver PPCF with education to the poor</t>
         </r>
       </text>
     </comment>
@@ -606,14 +648,14 @@
         </r>
       </text>
     </comment>
-    <comment ref="C21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0900-000009000000}">
+    <comment ref="C21" authorId="0" shapeId="0" xr:uid="{9BF08685-00AE-914A-9178-3CDB9EDE5066}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t>Sam:</t>
@@ -621,12 +663,21 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Fictional</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Assumed same as stunting</t>
         </r>
       </text>
     </comment>
@@ -1560,6 +1611,39 @@
           </rPr>
           <t xml:space="preserve">
 Probably can delete</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F7" authorId="0" shapeId="0" xr:uid="{9793A938-F8E3-8A4F-986E-078A459B470E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nick had RR in params doc, I fixed AF and solved for Eff</t>
         </r>
       </text>
     </comment>
@@ -4344,7 +4428,7 @@
     <numFmt numFmtId="166" formatCode="0.0000"/>
     <numFmt numFmtId="167" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -4543,6 +4627,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="14">
@@ -8204,7 +8301,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -8773,7 +8872,7 @@
   </sheetPr>
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="J61" sqref="J61"/>
     </sheetView>
   </sheetViews>
@@ -12830,12 +12929,14 @@
   </sheetPr>
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="36.6640625" customWidth="1"/>
-    <col min="2" max="2" width="64.5" customWidth="1"/>
+    <col min="2" max="2" width="76.33203125" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" customWidth="1"/>
     <col min="4" max="4" width="15.83203125" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" customWidth="1"/>
@@ -12897,19 +12998,19 @@
         <v>213</v>
       </c>
       <c r="C4">
-        <v>1.04</v>
+        <v>1.024</v>
       </c>
       <c r="D4">
-        <v>1.04</v>
+        <v>1.024</v>
       </c>
       <c r="E4">
-        <v>1.04</v>
+        <v>1.024</v>
       </c>
       <c r="F4">
-        <v>1.04</v>
+        <v>1.024</v>
       </c>
       <c r="G4">
-        <v>1.04</v>
+        <v>1.024</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
@@ -13057,12 +13158,10 @@
         <v>1</v>
       </c>
       <c r="E13" s="4">
-        <f>1/(1 + (E7-1)*(1-'Baseline year demographics'!$C$8))</f>
-        <v>0.76409370845240454</v>
+        <v>0.77</v>
       </c>
       <c r="F13" s="4">
-        <f>1/(1 + (F7-1)*(1-'Baseline year demographics'!$C$8))</f>
-        <v>0.76409370845240454</v>
+        <v>0.77</v>
       </c>
       <c r="G13" s="4">
         <v>1</v>
@@ -13079,12 +13178,10 @@
         <v>1</v>
       </c>
       <c r="E14" s="4">
-        <f>1 / (E$10/E$9)</f>
-        <v>0.66945606694560678</v>
+        <v>0.89</v>
       </c>
       <c r="F14" s="4">
-        <f>1 / (F$10/F$9)</f>
-        <v>0.66945606694560678</v>
+        <v>0.89</v>
       </c>
       <c r="G14" s="4">
         <v>1</v>
@@ -13101,12 +13198,10 @@
         <v>1</v>
       </c>
       <c r="E15" s="4">
-        <f t="shared" ref="E15:F16" si="0">1 / (E$10/E$9)</f>
-        <v>0.66945606694560678</v>
+        <v>0.89</v>
       </c>
       <c r="F15" s="4">
-        <f t="shared" si="0"/>
-        <v>0.66945606694560678</v>
+        <v>0.89</v>
       </c>
       <c r="G15" s="4">
         <v>1</v>
@@ -13123,12 +13218,10 @@
         <v>1</v>
       </c>
       <c r="E16" s="4">
-        <f t="shared" si="0"/>
-        <v>0.66945606694560678</v>
+        <v>0.89</v>
       </c>
       <c r="F16" s="4">
-        <f t="shared" si="0"/>
-        <v>0.66945606694560678</v>
+        <v>0.89</v>
       </c>
       <c r="G16" s="4">
         <v>1</v>
@@ -13186,20 +13279,20 @@
       <c r="B21" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="C21" s="44">
-        <v>1.04</v>
-      </c>
-      <c r="D21" s="44">
-        <v>1.04</v>
-      </c>
-      <c r="E21" s="44">
-        <v>1.04</v>
-      </c>
-      <c r="F21" s="44">
-        <v>1.04</v>
-      </c>
-      <c r="G21" s="44">
-        <v>1.04</v>
+      <c r="C21">
+        <v>1.024</v>
+      </c>
+      <c r="D21">
+        <v>1.024</v>
+      </c>
+      <c r="E21">
+        <v>1.024</v>
+      </c>
+      <c r="F21">
+        <v>1.024</v>
+      </c>
+      <c r="G21">
+        <v>1.024</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.15">
@@ -13209,20 +13302,20 @@
       <c r="B23" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="C23" s="44">
-        <v>1.04</v>
-      </c>
-      <c r="D23" s="44">
-        <v>1.04</v>
-      </c>
-      <c r="E23" s="44">
-        <v>1.04</v>
-      </c>
-      <c r="F23" s="44">
-        <v>1.04</v>
-      </c>
-      <c r="G23" s="44">
-        <v>1.04</v>
+      <c r="C23">
+        <v>1.024</v>
+      </c>
+      <c r="D23">
+        <v>1.024</v>
+      </c>
+      <c r="E23">
+        <v>1.024</v>
+      </c>
+      <c r="F23">
+        <v>1.024</v>
+      </c>
+      <c r="G23">
+        <v>1.024</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.15">
@@ -17368,7 +17461,9 @@
   </sheetPr>
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -17535,14 +17630,16 @@
       <c r="E7" s="45">
         <v>0</v>
       </c>
-      <c r="F7" s="45">
-        <v>0.62</v>
-      </c>
-      <c r="G7" s="45">
-        <v>0.62</v>
+      <c r="F7" s="12">
+        <f>1-(0.913+0.335-1)/0.335</f>
+        <v>0.25970149253731345</v>
+      </c>
+      <c r="G7" s="12">
+        <f>1-(0.913+0.335-1)/0.335</f>
+        <v>0.25970149253731345</v>
       </c>
       <c r="H7" s="45">
-        <v>0.62</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.15">
@@ -17578,14 +17675,16 @@
       <c r="E9" s="45">
         <v>0</v>
       </c>
-      <c r="F9" s="45">
-        <v>0.62</v>
-      </c>
-      <c r="G9" s="45">
-        <v>0.62</v>
+      <c r="F9" s="12">
+        <f>1-(0.913+0.335-1)/0.335</f>
+        <v>0.25970149253731345</v>
+      </c>
+      <c r="G9" s="12">
+        <f>1-(0.913+0.335-1)/0.335</f>
+        <v>0.25970149253731345</v>
       </c>
       <c r="H9" s="45">
-        <v>0.62</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.15">
@@ -17624,14 +17723,16 @@
       <c r="E11" s="45">
         <v>0</v>
       </c>
-      <c r="F11" s="45">
-        <v>0.62</v>
-      </c>
-      <c r="G11" s="45">
-        <v>0.62</v>
+      <c r="F11" s="12">
+        <f>1-(0.913+0.335-1)/0.335</f>
+        <v>0.25970149253731345</v>
+      </c>
+      <c r="G11" s="12">
+        <f>1-(0.913+0.335-1)/0.335</f>
+        <v>0.25970149253731345</v>
       </c>
       <c r="H11" s="45">
-        <v>0.62</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.15">
@@ -17667,14 +17768,16 @@
       <c r="E13" s="45">
         <v>0</v>
       </c>
-      <c r="F13" s="45">
-        <v>0.62</v>
-      </c>
-      <c r="G13" s="45">
-        <v>0.62</v>
+      <c r="F13" s="12">
+        <f>1-(0.913+0.335-1)/0.335</f>
+        <v>0.25970149253731345</v>
+      </c>
+      <c r="G13" s="12">
+        <f>1-(0.913+0.335-1)/0.335</f>
+        <v>0.25970149253731345</v>
       </c>
       <c r="H13" s="45">
-        <v>0.62</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.15">
@@ -17713,14 +17816,16 @@
       <c r="E15" s="45">
         <v>0</v>
       </c>
-      <c r="F15" s="45">
-        <v>0.62</v>
-      </c>
-      <c r="G15" s="45">
-        <v>0.62</v>
+      <c r="F15" s="12">
+        <f>1-(0.913+0.335-1)/0.335</f>
+        <v>0.25970149253731345</v>
+      </c>
+      <c r="G15" s="12">
+        <f>1-(0.913+0.335-1)/0.335</f>
+        <v>0.25970149253731345</v>
       </c>
       <c r="H15" s="45">
-        <v>0.62</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.15">
@@ -17756,14 +17861,16 @@
       <c r="E17" s="45">
         <v>0</v>
       </c>
-      <c r="F17" s="45">
-        <v>0.62</v>
-      </c>
-      <c r="G17" s="45">
-        <v>0.62</v>
+      <c r="F17" s="12">
+        <f>1-(0.913+0.335-1)/0.335</f>
+        <v>0.25970149253731345</v>
+      </c>
+      <c r="G17" s="12">
+        <f>1-(0.913+0.335-1)/0.335</f>
+        <v>0.25970149253731345</v>
       </c>
       <c r="H17" s="45">
-        <v>0.62</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.15">
@@ -19027,7 +19134,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O36" sqref="O36"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated effectiveness incidence for Vit A
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Tanzania/2018Jan/InputForCode_Tanzania.xlsx
+++ b/input_spreadsheets/Tanzania/2018Jan/InputForCode_Tanzania.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/input_spreadsheets/Tanzania/2018Jan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587EF0E9-8DFA-784A-B9D3-AE001601A0B5}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05694F9-C532-D446-8322-8E10995F2C58}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-21140" windowWidth="38400" windowHeight="21140" firstSheet="22" activeTab="25" xr2:uid="{9CA16DF4-3AE6-9240-921D-580CF0357D1B}"/>
+    <workbookView xWindow="0" yWindow="-21140" windowWidth="38400" windowHeight="21140" firstSheet="17" activeTab="19" xr2:uid="{9CA16DF4-3AE6-9240-921D-580CF0357D1B}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -17539,8 +17539,8 @@
   </sheetPr>
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="125" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -17642,13 +17642,16 @@
         <v>0</v>
       </c>
       <c r="F4" s="4">
-        <v>0.62</v>
+        <f>1-(0.871+F2-1)/F2</f>
+        <v>0.38507462686567184</v>
       </c>
       <c r="G4" s="4">
-        <v>0.62</v>
+        <f t="shared" ref="G4:H4" si="1">1-(0.871+G2-1)/G2</f>
+        <v>0.38507462686567184</v>
       </c>
       <c r="H4" s="4">
-        <v>0.62</v>
+        <f t="shared" si="1"/>
+        <v>0.38507462686567184</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
@@ -24031,7 +24034,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Removed FP from run
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Tanzania/2018Jan/InputForCode_Tanzania.xlsx
+++ b/input_spreadsheets/Tanzania/2018Jan/InputForCode_Tanzania.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/input_spreadsheets/Tanzania/2018Jan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05694F9-C532-D446-8322-8E10995F2C58}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A543966-2B25-CE46-8C0F-C999E97B3593}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-21140" windowWidth="38400" windowHeight="21140" firstSheet="17" activeTab="19" xr2:uid="{9CA16DF4-3AE6-9240-921D-580CF0357D1B}"/>
+    <workbookView xWindow="0" yWindow="-21140" windowWidth="38400" windowHeight="21140" firstSheet="23" activeTab="31" xr2:uid="{9CA16DF4-3AE6-9240-921D-580CF0357D1B}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -2053,7 +2053,7 @@
           <rPr>
             <b/>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
@@ -2062,12 +2062,21 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Exposed to malaria
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Exposed to malaria
 </t>
         </r>
       </text>
@@ -3130,7 +3139,7 @@
           <rPr>
             <b/>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
@@ -3139,12 +3148,21 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-From Jakub's book, annual incidence of severe acute wasting is annual prevalence * 1.6  (p. 147). Assuming the same to be true for moderate wasting.</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>From Jakub's book, annual incidence of severe acute wasting is annual prevalence * 1.6  (p. 147). Assuming the same to be true for moderate wasting.</t>
         </r>
       </text>
     </comment>
@@ -3622,7 +3640,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1487" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1486" uniqueCount="290">
   <si>
     <t>year</t>
   </si>
@@ -17539,8 +17557,8 @@
   </sheetPr>
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -27604,8 +27622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -27656,9 +27674,7 @@
       <c r="A6" t="s">
         <v>185</v>
       </c>
-      <c r="B6" s="133" t="s">
-        <v>165</v>
-      </c>
+      <c r="B6" s="133"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" s="12" t="s">
@@ -28927,7 +28943,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>

</xml_diff>

<commit_message>
Adjusted progs to include
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Tanzania/2018Jan/InputForCode_Tanzania.xlsx
+++ b/input_spreadsheets/Tanzania/2018Jan/InputForCode_Tanzania.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/input_spreadsheets/Tanzania/2018Jan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5C7EC08-B28E-C847-A8DA-0F9B61F50115}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B98DD7BD-A0C9-7943-89B6-7D1BD4D528AC}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38200" yWindow="-21140" windowWidth="38400" windowHeight="21140" firstSheet="22" activeTab="27" xr2:uid="{9CA16DF4-3AE6-9240-921D-580CF0357D1B}"/>
+    <workbookView xWindow="-38200" yWindow="-21140" windowWidth="38400" windowHeight="21140" firstSheet="22" activeTab="31" xr2:uid="{9CA16DF4-3AE6-9240-921D-580CF0357D1B}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -3724,7 +3724,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1433" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1465" uniqueCount="285">
   <si>
     <t>year</t>
   </si>
@@ -24799,7 +24799,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
@@ -27446,8 +27446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -27468,7 +27468,9 @@
       <c r="A2" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="133"/>
+      <c r="B2" s="133" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" s="120" t="s">
@@ -27488,7 +27490,9 @@
       <c r="A5" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B5" s="133"/>
+      <c r="B5" s="133" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
@@ -27500,7 +27504,9 @@
       <c r="A7" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="B7" s="133"/>
+      <c r="B7" s="133" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" s="12" t="s">
@@ -27524,7 +27530,9 @@
       <c r="A11" t="s">
         <v>128</v>
       </c>
-      <c r="B11" s="133"/>
+      <c r="B11" s="133" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
@@ -27536,7 +27544,9 @@
       <c r="A13" t="s">
         <v>129</v>
       </c>
-      <c r="B13" s="133"/>
+      <c r="B13" s="133" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
@@ -27548,7 +27558,9 @@
       <c r="A15" t="s">
         <v>130</v>
       </c>
-      <c r="B15" s="133"/>
+      <c r="B15" s="133" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
@@ -27560,7 +27572,9 @@
       <c r="A17" t="s">
         <v>127</v>
       </c>
-      <c r="B17" s="133"/>
+      <c r="B17" s="133" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
@@ -27572,7 +27586,9 @@
       <c r="A19" t="s">
         <v>125</v>
       </c>
-      <c r="B19" s="133"/>
+      <c r="B19" s="133" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
@@ -27584,7 +27600,9 @@
       <c r="A21" t="s">
         <v>126</v>
       </c>
-      <c r="B21" s="133"/>
+      <c r="B21" s="133" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
@@ -27596,13 +27614,17 @@
       <c r="A23" t="s">
         <v>124</v>
       </c>
-      <c r="B23" s="133"/>
+      <c r="B23" s="133" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>115</v>
       </c>
-      <c r="B24" s="133"/>
+      <c r="B24" s="133" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" s="4" t="s">
@@ -27614,29 +27636,41 @@
       <c r="A26" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="B26" s="133"/>
+      <c r="B26" s="133" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B27" s="133"/>
+      <c r="B27" s="133" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="s">
         <v>77</v>
       </c>
+      <c r="B28" s="133" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A29" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="B29" s="133"/>
+      <c r="B29" s="133" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A30" s="4" t="s">
         <v>261</v>
       </c>
+      <c r="B30" s="133" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
@@ -27647,17 +27681,25 @@
       <c r="A32" t="s">
         <v>134</v>
       </c>
+      <c r="B32" s="133" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>258</v>
       </c>
+      <c r="B33" s="133" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A34" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B34" s="133"/>
+      <c r="B34" s="133" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A35" s="4" t="s">
@@ -27668,6 +27710,9 @@
       <c r="A36" s="4" t="s">
         <v>132</v>
       </c>
+      <c r="B36" s="133" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A37" s="4" t="s">
@@ -27678,69 +27723,104 @@
       <c r="A38" s="29" t="s">
         <v>133</v>
       </c>
+      <c r="B38" s="133" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A39" s="4" t="s">
         <v>147</v>
       </c>
+      <c r="B39" s="133" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="s">
         <v>148</v>
       </c>
+      <c r="B40" s="133" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A41" s="4" t="s">
         <v>47</v>
       </c>
+      <c r="B41" s="133" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>257</v>
       </c>
+      <c r="B42" s="133" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>256</v>
       </c>
+      <c r="B43" s="133" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
         <v>255</v>
       </c>
+      <c r="B44" s="133" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
         <v>253</v>
       </c>
+      <c r="B45" s="133" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
         <v>254</v>
       </c>
+      <c r="B46" s="133" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
         <v>259</v>
       </c>
+      <c r="B47" s="133" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A48" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="B48" s="133"/>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B48" s="133" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A49" s="11" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B49" s="133" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A50" s="11" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A51" s="11" t="s">
         <v>159</v>
       </c>

</xml_diff>

<commit_message>
Changed saturation con to 95%
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Tanzania/2018Jan/InputForCode_Tanzania.xlsx
+++ b/input_spreadsheets/Tanzania/2018Jan/InputForCode_Tanzania.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/input_spreadsheets/Tanzania/2018Jan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B98DD7BD-A0C9-7943-89B6-7D1BD4D528AC}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7D7F3D5-7CFE-464A-9B4D-1B1C2E86F335}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38200" yWindow="-21140" windowWidth="38400" windowHeight="21140" firstSheet="22" activeTab="31" xr2:uid="{9CA16DF4-3AE6-9240-921D-580CF0357D1B}"/>
+    <workbookView xWindow="-38760" yWindow="-18760" windowWidth="38400" windowHeight="21140" firstSheet="22" activeTab="28" xr2:uid="{9CA16DF4-3AE6-9240-921D-580CF0357D1B}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -2478,7 +2478,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
@@ -2487,12 +2487,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-This is the fraction of the population eating these staples and belongs here.</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>This is the fraction of the population eating these staples and belongs here.</t>
         </r>
       </text>
     </comment>
@@ -2847,7 +2856,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
@@ -2856,13 +2865,31 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-made up
-Janka: add $1 as cost of sprinkles</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">made up
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Janka: add $1 as cost of sprinkles</t>
         </r>
       </text>
     </comment>
@@ -4592,7 +4619,7 @@
     <numFmt numFmtId="166" formatCode="0.0000"/>
     <numFmt numFmtId="167" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="37" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -4816,6 +4843,19 @@
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -25099,8 +25139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -25147,7 +25187,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="126">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D3" s="126">
         <v>0.8</v>
@@ -25161,7 +25201,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="126">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D4" s="126">
         <v>7</v>
@@ -25175,7 +25215,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="126">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D5" s="126">
         <f>180</f>
@@ -25190,7 +25230,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="126">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D6" s="126">
         <f>SUM('Programs family planning'!E2:E10)</f>
@@ -25219,7 +25259,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="126">
-        <v>0.8</v>
+        <v>0.95</v>
       </c>
       <c r="D8" s="126">
         <v>0.75</v>
@@ -25233,7 +25273,7 @@
         <v>0</v>
       </c>
       <c r="C9" s="126">
-        <v>0.12</v>
+        <v>0.95</v>
       </c>
       <c r="D9" s="126">
         <v>0.19</v>
@@ -25247,7 +25287,7 @@
         <v>0</v>
       </c>
       <c r="C10" s="126">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D10" s="126">
         <v>0.73</v>
@@ -25261,7 +25301,7 @@
         <v>0</v>
       </c>
       <c r="C11" s="126">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D11" s="126">
         <v>0.73</v>
@@ -25275,7 +25315,7 @@
         <v>0</v>
       </c>
       <c r="C12" s="126">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D12" s="126">
         <v>1.78</v>
@@ -25289,7 +25329,7 @@
         <v>0</v>
       </c>
       <c r="C13" s="126">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D13" s="126">
         <v>1.78</v>
@@ -25303,7 +25343,7 @@
         <v>0</v>
       </c>
       <c r="C14" s="126">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D14" s="126">
         <v>0.24</v>
@@ -25317,7 +25357,7 @@
         <v>0</v>
       </c>
       <c r="C15" s="126">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D15" s="126">
         <v>0.24</v>
@@ -25331,7 +25371,7 @@
         <v>0</v>
       </c>
       <c r="C16" s="126">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D16" s="126">
         <v>0.55000000000000004</v>
@@ -25345,7 +25385,7 @@
         <v>0</v>
       </c>
       <c r="C17" s="126">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D17" s="126">
         <v>0.55000000000000004</v>
@@ -25359,7 +25399,7 @@
         <v>0</v>
       </c>
       <c r="C18" s="126">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D18" s="126">
         <v>0.73</v>
@@ -25373,7 +25413,7 @@
         <v>0</v>
       </c>
       <c r="C19" s="126">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D19" s="126">
         <v>0.73</v>
@@ -25387,7 +25427,7 @@
         <v>0</v>
       </c>
       <c r="C20" s="126">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D20" s="126">
         <v>1.78</v>
@@ -25401,7 +25441,7 @@
         <v>0</v>
       </c>
       <c r="C21" s="126">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D21" s="126">
         <v>1.78</v>
@@ -25415,7 +25455,7 @@
         <v>0</v>
       </c>
       <c r="C22" s="126">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D22" s="126">
         <v>0.55000000000000004</v>
@@ -25429,7 +25469,7 @@
         <v>0</v>
       </c>
       <c r="C23" s="126">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D23" s="126">
         <v>0.55000000000000004</v>
@@ -25457,7 +25497,7 @@
         <v>0</v>
       </c>
       <c r="C25" s="126">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D25" s="126">
         <v>1.78</v>
@@ -25471,7 +25511,7 @@
         <v>0</v>
       </c>
       <c r="C26" s="126">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D26" s="126">
         <v>1.78</v>
@@ -25513,7 +25553,7 @@
         <v>0</v>
       </c>
       <c r="C29" s="126">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D29" s="126">
         <v>11</v>
@@ -25527,7 +25567,7 @@
         <v>0</v>
       </c>
       <c r="C30" s="126">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D30" s="126">
         <v>11</v>
@@ -25541,7 +25581,7 @@
         <v>0</v>
       </c>
       <c r="C31" s="126">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D31" s="126">
         <v>2.99</v>
@@ -25569,7 +25609,7 @@
         <v>0</v>
       </c>
       <c r="C33" s="126">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D33" s="126">
         <v>23.84</v>
@@ -25597,7 +25637,7 @@
         <v>0</v>
       </c>
       <c r="C35" s="126">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D35" s="126">
         <v>50</v>
@@ -25611,7 +25651,7 @@
         <v>0</v>
       </c>
       <c r="C36" s="126">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D36" s="126">
         <v>51</v>
@@ -25625,7 +25665,7 @@
         <v>0</v>
       </c>
       <c r="C37" s="126">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D37" s="126">
         <v>4.6500000000000004</v>
@@ -25781,7 +25821,7 @@
         <v>0</v>
       </c>
       <c r="C48" s="126">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="D48" s="126">
         <v>4</v>
@@ -27446,7 +27486,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated progs for run
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Tanzania/2018Jan/InputForCode_Tanzania.xlsx
+++ b/input_spreadsheets/Tanzania/2018Jan/InputForCode_Tanzania.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/input_spreadsheets/Tanzania/2018Jan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7D7F3D5-7CFE-464A-9B4D-1B1C2E86F335}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1498F10D-0CA0-6F45-8BD2-105C9ED685B6}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38760" yWindow="-18760" windowWidth="38400" windowHeight="21140" firstSheet="22" activeTab="28" xr2:uid="{9CA16DF4-3AE6-9240-921D-580CF0357D1B}"/>
+    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" firstSheet="22" activeTab="28" xr2:uid="{9CA16DF4-3AE6-9240-921D-580CF0357D1B}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -3751,7 +3751,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1465" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1460" uniqueCount="285">
   <si>
     <t>year</t>
   </si>
@@ -25139,8 +25139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -25245,7 +25245,7 @@
         <v>0.36</v>
       </c>
       <c r="C7" s="123">
-        <v>0.8</v>
+        <v>0.95</v>
       </c>
       <c r="D7" s="123">
         <v>0.25</v>
@@ -27487,7 +27487,7 @@
   <dimension ref="A1:B51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -27795,41 +27795,31 @@
       <c r="A42" t="s">
         <v>257</v>
       </c>
-      <c r="B42" s="133" t="s">
-        <v>161</v>
-      </c>
+      <c r="B42" s="133"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>256</v>
       </c>
-      <c r="B43" s="133" t="s">
-        <v>161</v>
-      </c>
+      <c r="B43" s="133"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
         <v>255</v>
       </c>
-      <c r="B44" s="133" t="s">
-        <v>161</v>
-      </c>
+      <c r="B44" s="133"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
         <v>253</v>
       </c>
-      <c r="B45" s="133" t="s">
-        <v>161</v>
-      </c>
+      <c r="B45" s="133"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
         <v>254</v>
       </c>
-      <c r="B46" s="133" t="s">
-        <v>161</v>
-      </c>
+      <c r="B46" s="133"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A47" t="s">

</xml_diff>